<commit_message>
Se agrega en el streamlit la info de competencias
</commit_message>
<xml_diff>
--- a/Competencias_Elasticidades.xlsx
+++ b/Competencias_Elasticidades.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rroldan\Documents\Layout Puebas Elasticidades\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F68B7BF1-94BB-43EB-B0DE-53D1F7153CD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B36520C-CDED-4468-B758-35F2D51481F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2500" yWindow="2500" windowWidth="19200" windowHeight="11170" xr2:uid="{947940E2-7CD9-41B7-8D9B-D7AAEE523B32}"/>
+    <workbookView xWindow="5040" yWindow="2160" windowWidth="16320" windowHeight="11170" xr2:uid="{947940E2-7CD9-41B7-8D9B-D7AAEE523B32}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -428,14 +428,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9FDEA1B3-2C93-402A-9F5A-DFB5771BAEB5}">
   <dimension ref="A1:E148"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+    <sheetView tabSelected="1" topLeftCell="A104" workbookViewId="0">
+      <selection activeCell="C106" sqref="C106:C148"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="12.81640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="22" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.7265625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2249,7 +2250,7 @@
         <v>3</v>
       </c>
       <c r="C107">
-        <v>2024</v>
+        <v>2025</v>
       </c>
       <c r="D107">
         <v>2</v>
@@ -2266,7 +2267,7 @@
         <v>3</v>
       </c>
       <c r="C108">
-        <v>2024</v>
+        <v>2025</v>
       </c>
       <c r="D108">
         <v>3</v>
@@ -2283,7 +2284,7 @@
         <v>3</v>
       </c>
       <c r="C109">
-        <v>2024</v>
+        <v>2025</v>
       </c>
       <c r="D109">
         <v>4</v>
@@ -2300,7 +2301,7 @@
         <v>3</v>
       </c>
       <c r="C110">
-        <v>2024</v>
+        <v>2025</v>
       </c>
       <c r="D110">
         <v>5</v>
@@ -2317,7 +2318,7 @@
         <v>3</v>
       </c>
       <c r="C111">
-        <v>2024</v>
+        <v>2025</v>
       </c>
       <c r="D111">
         <v>6</v>
@@ -2334,7 +2335,7 @@
         <v>3</v>
       </c>
       <c r="C112">
-        <v>2024</v>
+        <v>2025</v>
       </c>
       <c r="D112">
         <v>7</v>
@@ -2351,7 +2352,7 @@
         <v>3</v>
       </c>
       <c r="C113">
-        <v>2024</v>
+        <v>2025</v>
       </c>
       <c r="D113">
         <v>8</v>
@@ -2368,7 +2369,7 @@
         <v>3</v>
       </c>
       <c r="C114">
-        <v>2024</v>
+        <v>2025</v>
       </c>
       <c r="D114">
         <v>9</v>
@@ -2385,7 +2386,7 @@
         <v>3</v>
       </c>
       <c r="C115">
-        <v>2024</v>
+        <v>2025</v>
       </c>
       <c r="D115">
         <v>10</v>
@@ -2402,7 +2403,7 @@
         <v>3</v>
       </c>
       <c r="C116">
-        <v>2024</v>
+        <v>2025</v>
       </c>
       <c r="D116">
         <v>11</v>
@@ -2419,7 +2420,7 @@
         <v>3</v>
       </c>
       <c r="C117">
-        <v>2024</v>
+        <v>2025</v>
       </c>
       <c r="D117">
         <v>12</v>
@@ -2436,7 +2437,7 @@
         <v>3</v>
       </c>
       <c r="C118">
-        <v>2024</v>
+        <v>2025</v>
       </c>
       <c r="D118">
         <v>13</v>
@@ -2453,7 +2454,7 @@
         <v>3</v>
       </c>
       <c r="C119">
-        <v>2024</v>
+        <v>2025</v>
       </c>
       <c r="D119">
         <v>14</v>
@@ -2470,7 +2471,7 @@
         <v>3</v>
       </c>
       <c r="C120">
-        <v>2024</v>
+        <v>2025</v>
       </c>
       <c r="D120">
         <v>15</v>
@@ -2487,7 +2488,7 @@
         <v>3</v>
       </c>
       <c r="C121">
-        <v>2024</v>
+        <v>2025</v>
       </c>
       <c r="D121">
         <v>16</v>
@@ -2504,7 +2505,7 @@
         <v>3</v>
       </c>
       <c r="C122">
-        <v>2024</v>
+        <v>2025</v>
       </c>
       <c r="D122">
         <v>17</v>
@@ -2521,7 +2522,7 @@
         <v>3</v>
       </c>
       <c r="C123">
-        <v>2024</v>
+        <v>2025</v>
       </c>
       <c r="D123">
         <v>18</v>
@@ -2538,7 +2539,7 @@
         <v>3</v>
       </c>
       <c r="C124">
-        <v>2024</v>
+        <v>2025</v>
       </c>
       <c r="D124">
         <v>19</v>
@@ -2555,7 +2556,7 @@
         <v>3</v>
       </c>
       <c r="C125">
-        <v>2024</v>
+        <v>2025</v>
       </c>
       <c r="D125">
         <v>20</v>
@@ -2572,7 +2573,7 @@
         <v>3</v>
       </c>
       <c r="C126">
-        <v>2024</v>
+        <v>2025</v>
       </c>
       <c r="D126">
         <v>21</v>
@@ -2589,7 +2590,7 @@
         <v>3</v>
       </c>
       <c r="C127">
-        <v>2024</v>
+        <v>2025</v>
       </c>
       <c r="D127">
         <v>22</v>
@@ -2606,7 +2607,7 @@
         <v>3</v>
       </c>
       <c r="C128">
-        <v>2024</v>
+        <v>2025</v>
       </c>
       <c r="D128">
         <v>23</v>
@@ -2623,7 +2624,7 @@
         <v>3</v>
       </c>
       <c r="C129">
-        <v>2024</v>
+        <v>2025</v>
       </c>
       <c r="D129">
         <v>24</v>
@@ -2640,7 +2641,7 @@
         <v>3</v>
       </c>
       <c r="C130">
-        <v>2024</v>
+        <v>2025</v>
       </c>
       <c r="D130">
         <v>25</v>
@@ -2657,7 +2658,7 @@
         <v>3</v>
       </c>
       <c r="C131">
-        <v>2024</v>
+        <v>2025</v>
       </c>
       <c r="D131">
         <v>26</v>
@@ -2674,7 +2675,7 @@
         <v>3</v>
       </c>
       <c r="C132">
-        <v>2024</v>
+        <v>2025</v>
       </c>
       <c r="D132">
         <v>27</v>
@@ -2691,7 +2692,7 @@
         <v>3</v>
       </c>
       <c r="C133">
-        <v>2024</v>
+        <v>2025</v>
       </c>
       <c r="D133">
         <v>28</v>
@@ -2708,7 +2709,7 @@
         <v>3</v>
       </c>
       <c r="C134">
-        <v>2024</v>
+        <v>2025</v>
       </c>
       <c r="D134">
         <v>29</v>
@@ -2725,7 +2726,7 @@
         <v>3</v>
       </c>
       <c r="C135">
-        <v>2024</v>
+        <v>2025</v>
       </c>
       <c r="D135">
         <v>30</v>
@@ -2742,7 +2743,7 @@
         <v>3</v>
       </c>
       <c r="C136">
-        <v>2024</v>
+        <v>2025</v>
       </c>
       <c r="D136">
         <v>31</v>
@@ -2759,7 +2760,7 @@
         <v>3</v>
       </c>
       <c r="C137">
-        <v>2024</v>
+        <v>2025</v>
       </c>
       <c r="D137">
         <v>32</v>
@@ -2776,7 +2777,7 @@
         <v>3</v>
       </c>
       <c r="C138">
-        <v>2024</v>
+        <v>2025</v>
       </c>
       <c r="D138">
         <v>33</v>
@@ -2793,7 +2794,7 @@
         <v>3</v>
       </c>
       <c r="C139">
-        <v>2024</v>
+        <v>2025</v>
       </c>
       <c r="D139">
         <v>34</v>
@@ -2810,7 +2811,7 @@
         <v>3</v>
       </c>
       <c r="C140">
-        <v>2024</v>
+        <v>2025</v>
       </c>
       <c r="D140">
         <v>35</v>
@@ -2827,7 +2828,7 @@
         <v>3</v>
       </c>
       <c r="C141">
-        <v>2024</v>
+        <v>2025</v>
       </c>
       <c r="D141">
         <v>36</v>
@@ -2844,7 +2845,7 @@
         <v>3</v>
       </c>
       <c r="C142">
-        <v>2024</v>
+        <v>2025</v>
       </c>
       <c r="D142">
         <v>37</v>
@@ -2861,7 +2862,7 @@
         <v>3</v>
       </c>
       <c r="C143">
-        <v>2024</v>
+        <v>2025</v>
       </c>
       <c r="D143">
         <v>38</v>
@@ -2878,7 +2879,7 @@
         <v>3</v>
       </c>
       <c r="C144">
-        <v>2024</v>
+        <v>2025</v>
       </c>
       <c r="D144">
         <v>39</v>
@@ -2895,7 +2896,7 @@
         <v>3</v>
       </c>
       <c r="C145">
-        <v>2024</v>
+        <v>2025</v>
       </c>
       <c r="D145">
         <v>40</v>
@@ -2912,7 +2913,7 @@
         <v>3</v>
       </c>
       <c r="C146">
-        <v>2024</v>
+        <v>2025</v>
       </c>
       <c r="D146">
         <v>41</v>
@@ -2929,7 +2930,7 @@
         <v>3</v>
       </c>
       <c r="C147">
-        <v>2024</v>
+        <v>2025</v>
       </c>
       <c r="D147">
         <v>42</v>
@@ -2946,7 +2947,7 @@
         <v>3</v>
       </c>
       <c r="C148">
-        <v>2024</v>
+        <v>2025</v>
       </c>
       <c r="D148">
         <v>43</v>

</xml_diff>